<commit_message>
Cambios Generales Junio 2024
</commit_message>
<xml_diff>
--- a/SistemaVentasBatia/Layouts/LayoutPlantilla.xlsx
+++ b/SistemaVentasBatia/Layouts/LayoutPlantilla.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAP_Sistemas5\source\repos\Ventas\SistemaVentasBatia\Layouts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDFE3EFE-695D-478D-970B-978FA78137D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61655EA3-2520-4BCD-B610-0DCEFFDD0BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30" yWindow="345" windowWidth="28770" windowHeight="10860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plantilla" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>Dia fin</t>
   </si>
@@ -92,6 +92,9 @@
   </si>
   <si>
     <t>Cubredescanso(1:SI,0:No)</t>
+  </si>
+  <si>
+    <t>Incluye Producto(1:SI,0:No)</t>
   </si>
 </sst>
 </file>
@@ -457,10 +460,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:U2"/>
+  <dimension ref="A1:V2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -482,9 +485,10 @@
     <col min="18" max="18" width="17.7109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="20" max="21" width="24" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="24.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -548,8 +552,11 @@
       <c r="U1" s="4" t="s">
         <v>21</v>
       </c>
+      <c r="V1" s="4" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
@@ -575,8 +582,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E919B3-B780-4274-AF92-1A2CD856599F}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Tipo de industria OK
</commit_message>
<xml_diff>
--- a/SistemaVentasBatia/Layouts/LayoutPlantilla.xlsx
+++ b/SistemaVentasBatia/Layouts/LayoutPlantilla.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAP_Sistemas5\source\repos\Ventas\SistemaVentasBatia\Layouts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61655EA3-2520-4BCD-B610-0DCEFFDD0BEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D15D4C4-BF95-4625-84DA-19210ECAEF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -463,7 +463,7 @@
   <dimension ref="A1:V2"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="U2" sqref="U2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
CAMBIOS ELSI, linea negocio,propuestas
</commit_message>
<xml_diff>
--- a/SistemaVentasBatia/Layouts/LayoutPlantilla.xlsx
+++ b/SistemaVentasBatia/Layouts/LayoutPlantilla.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAP_Sistemas5\source\repos\Ventas\SistemaVentasBatia\Layouts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D15D4C4-BF95-4625-84DA-19210ECAEF91}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E55EA460-1648-447F-B5FB-C55E7D5708D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="23">
   <si>
     <t>Dia fin</t>
   </si>
@@ -580,26 +580,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8E919B3-B780-4274-AF92-1A2CD856599F}">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="50.28515625" customWidth="1"/>
+    <col min="3" max="3" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>10</v>
       </c>
       <c r="B1" s="3" t="s">
         <v>9</v>
       </c>
+      <c r="C1" s="4" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B2" s="2"/>
     </row>
   </sheetData>

</xml_diff>